<commit_message>
Changed config file. Modified reading from file, but needs to improve
</commit_message>
<xml_diff>
--- a/PWC. Шаблоны входа робота.xlsx
+++ b/PWC. Шаблоны входа робота.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vietnguyen/Dropbox/Share/PWC. Robotics/Aeroflot/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\PwC\PwC-Aeroflot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13DBCE5-2326-3B41-B935-F86A8726BB58}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D527939-193B-4938-9E56-600B92B678B2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4640" yWindow="460" windowWidth="28800" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4644" yWindow="456" windowWidth="28800" windowHeight="15984" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
+    <sheet name="Инструкция" sheetId="5" r:id="rId1"/>
+    <sheet name="Params" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="114">
   <si>
     <t>Расстояние</t>
   </si>
@@ -140,13 +141,240 @@
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>Код робота</t>
+  </si>
+  <si>
+    <t>R2 (Тест + Аналитика)</t>
+  </si>
+  <si>
+    <t>Описание робота</t>
+  </si>
+  <si>
+    <t>Ипользуемые транзакции SAP</t>
+  </si>
+  <si>
+    <t>Как запустить робота?</t>
+  </si>
+  <si>
+    <t>Входные данные</t>
+  </si>
+  <si>
+    <t>При запуске робота необходимо обеспечить наличие следующих данных:</t>
+  </si>
+  <si>
+    <t>Инструкция по заполнению конфигурационного файла</t>
+  </si>
+  <si>
+    <t>..</t>
+  </si>
+  <si>
+    <t>Описание шагов робота</t>
+  </si>
+  <si>
+    <t>Код шага</t>
+  </si>
+  <si>
+    <t>Краткое наименование шага</t>
+  </si>
+  <si>
+    <t>Точка входа</t>
+  </si>
+  <si>
+    <t>Точка выхода</t>
+  </si>
+  <si>
+    <t>Признак: разработано?</t>
+  </si>
+  <si>
+    <t>Краткое описание шага</t>
+  </si>
+  <si>
+    <t>STReadConfiguration</t>
+  </si>
+  <si>
+    <t>Выполнить чтение конфигурации</t>
+  </si>
+  <si>
+    <t>Рабочий стол</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>Выполнить загрузку конфигурационного файла в переменные</t>
+  </si>
+  <si>
+    <t>STValidateConfiguration</t>
+  </si>
+  <si>
+    <t>Выполнить валидацию входящих данных</t>
+  </si>
+  <si>
+    <t>Выполнить всевозможную валидацию всего, что только можно: проверить наличие всех входных/выходных файлов и папок. Проверить структуры ОСВ и т.д.</t>
+  </si>
+  <si>
+    <t>STPrepareStatus</t>
+  </si>
+  <si>
+    <t>Выполнить формирование статусного файла</t>
+  </si>
+  <si>
+    <t>Сформировать рыбу статусного файла Status.xlsm, который должен лежать в корне Output folder. Внимание: При формировании статусного файла используется VBA код (STPrepareStatus), хранимый в конфигурационном файле.</t>
+  </si>
+  <si>
+    <t>AOpenSAP</t>
+  </si>
+  <si>
+    <t>Выполнить вход в SAP</t>
+  </si>
+  <si>
+    <t>Главное меню SAP</t>
+  </si>
+  <si>
+    <t>STProcessRow</t>
+  </si>
+  <si>
+    <t>Циклическая отработка строк конфигурации</t>
+  </si>
+  <si>
+    <t>Выполнить обработку строки конфигурации: подготовить файловую структуру, запустить процесс циклической технической выгрузки
+Сформировать/проверить наличие папки группы
+Сформировать/проверить наличие файла выгрузки</t>
+  </si>
+  <si>
+    <t>STProcessRowSTExportSAP</t>
+  </si>
+  <si>
+    <t>Циклическая выгрузка технических файликов</t>
+  </si>
+  <si>
+    <t>STProcessRowSTExportSAPAExportPart</t>
+  </si>
+  <si>
+    <t>Выполнить выгрузку части данных</t>
+  </si>
+  <si>
+    <t>Зайти в транзакцию, установить параметры, запустить формирование, выполнить экспорт и сохранить Excel файл на диск</t>
+  </si>
+  <si>
+    <t>STProcessRowACombineTechPart</t>
+  </si>
+  <si>
+    <t>Добавить выгруженные данные в основной файл</t>
+  </si>
+  <si>
+    <t>Выполнить объединение технических файлов в один.+Подтягивание списка ВГО контрагентов. +Подтягивание ОСВ. При выполнении операции используется VBA код STProcessRowACombineTechPart</t>
+  </si>
+  <si>
+    <t>STProcessRowARecalculateRowFile</t>
+  </si>
+  <si>
+    <t>Выполнить обсчет файла</t>
+  </si>
+  <si>
+    <t>Выполнить расчет Excel файла: расчет доп. колонок в выгрузке; расчет доп. Колонки в ОСВ (код счета); Обновлние пивота ОСВСвод; Обновление пивота Сверка; Обновление пивота Свод   При выполнении операции используется VBA код STProcessRowARecalculateRowFile</t>
+  </si>
+  <si>
+    <t>STProcessGroup</t>
+  </si>
+  <si>
+    <t>Циклическая отработка групп</t>
+  </si>
+  <si>
+    <t>STProcessGroupAUpdateGroupFile</t>
+  </si>
+  <si>
+    <t>Сформировать/проверить файл группы</t>
+  </si>
+  <si>
+    <t>STProcessGroupSTProcessRowFile</t>
+  </si>
+  <si>
+    <t>Циклическая обработка основных файлов группы</t>
+  </si>
+  <si>
+    <t>STProcessGroupSTProcessRowFileAAddToGroupFile</t>
+  </si>
+  <si>
+    <t>Скопировать данные из вкладки Свод основного файла строки и добавить в конец вкладки Свод файла группы</t>
+  </si>
+  <si>
+    <t>STProcessGroupSTProcessRowFileAProcessGroupFile</t>
+  </si>
+  <si>
+    <t>Обработать групповой файл</t>
+  </si>
+  <si>
+    <t>STPrepareStatusASetData</t>
+  </si>
+  <si>
+    <t>Вывести информацию о статусе обработки в файл</t>
+  </si>
+  <si>
+    <t>ACloseSAP</t>
+  </si>
+  <si>
+    <t>Закрыть SAP</t>
+  </si>
+  <si>
+    <t>Закрыть приложение SAP</t>
+  </si>
+  <si>
+    <t>ADisconnectVPN</t>
+  </si>
+  <si>
+    <t>Выключить VPN</t>
+  </si>
+  <si>
+    <t>Закрыть VPN соединение</t>
+  </si>
+  <si>
+    <t>AConnectVPN</t>
+  </si>
+  <si>
+    <t>Включить VPN</t>
+  </si>
+  <si>
+    <t>Открыть VPN соединение</t>
+  </si>
+  <si>
+    <t>AConnectWiFi</t>
+  </si>
+  <si>
+    <t>Включить WiFi</t>
+  </si>
+  <si>
+    <t>Открыть WiFi соединение</t>
+  </si>
+  <si>
+    <t>TEstablishConnection</t>
+  </si>
+  <si>
+    <t>Установка соединения</t>
+  </si>
+  <si>
+    <t>Установить необходимое соединение (на случай, если наблюдаются проблемы с доступом)</t>
+  </si>
+  <si>
+    <t>Заходим на сайт "Аэрофлота" https://www.aeroflot.ru/ikm/, вводим данные о перелетах по направлениям из входного файла, считываем данные о бонусныхбаллах за данные перелеты и сохраняем в выходной файл</t>
+  </si>
+  <si>
+    <t>файл конфигурации в формате *.xlsx</t>
+  </si>
+  <si>
+    <t>Перед запуском рекомендуется закрыть все окна Excel и Chrome. После запуска робот самостоятельно выполнит следующие действия: откроет конфигурационный файл Excel, прочитает входные параметры, откроет страницу браузера на сайте компании "Аэрофлот", выполнит выгрузку данных с сайта, обработает данные и сохранит результат работы в Excel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -174,6 +402,96 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="5"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="5"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -195,7 +513,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -283,11 +601,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -326,9 +659,63 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
@@ -644,9 +1031,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -684,7 +1071,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -790,7 +1177,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -939,6 +1326,538 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39BFAB1C-68A9-4038-9886-24B2DD8AE8D1}">
+  <dimension ref="A1:F30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.88671875" customWidth="1"/>
+    <col min="2" max="2" width="35.21875" customWidth="1"/>
+    <col min="3" max="3" width="25.109375" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+    <col min="5" max="5" width="23.44140625" customWidth="1"/>
+    <col min="6" max="6" width="35.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+    </row>
+    <row r="2" spans="1:6" ht="51" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+    </row>
+    <row r="4" spans="1:6" ht="82.2" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+    </row>
+    <row r="5" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="35"/>
+      <c r="B6" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+    </row>
+    <row r="7" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="19"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A12" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="61.8" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="51.6" x14ac:dyDescent="0.25">
+      <c r="A15" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="23"/>
+    </row>
+    <row r="17" spans="1:6" ht="31.2" x14ac:dyDescent="0.25">
+      <c r="A17" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="51.6" x14ac:dyDescent="0.25">
+      <c r="A18" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="61.8" x14ac:dyDescent="0.25">
+      <c r="A19" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="31"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="23"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="23"/>
+    </row>
+    <row r="23" spans="1:6" ht="31.2" x14ac:dyDescent="0.25">
+      <c r="A23" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="E23" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="23"/>
+    </row>
+    <row r="24" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A24" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="23"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="E25" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="23"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="F26" s="26" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="F27" s="26" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="B28" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E28" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="F28" s="26" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E29" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="F29" s="26" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A30" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="B30" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="C30" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E30" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="F30" s="26" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A5:A6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -949,19 +1868,19 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
     <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -987,7 +1906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -1013,7 +1932,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
@@ -1039,7 +1958,7 @@
         <v>11506</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
@@ -1055,7 +1974,7 @@
       <c r="G4" s="16"/>
       <c r="H4" s="12"/>
     </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>1</v>
       </c>
@@ -1081,7 +2000,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>35</v>
       </c>
@@ -1105,7 +2024,7 @@
       </c>
       <c r="H6" s="12"/>
     </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>1</v>
       </c>
@@ -1129,7 +2048,7 @@
       </c>
       <c r="H7" s="12"/>
     </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>1</v>
       </c>
@@ -1153,7 +2072,7 @@
       </c>
       <c r="H8" s="12"/>
     </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>1</v>
       </c>
@@ -1179,7 +2098,7 @@
         <v>24484</v>
       </c>
     </row>
-    <row r="20" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -1190,7 +2109,7 @@
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
     </row>
-    <row r="21" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F21" s="3"/>
       <c r="G21" s="4"/>
       <c r="H21" s="5"/>
@@ -1201,7 +2120,7 @@
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
     </row>
-    <row r="22" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -1212,7 +2131,7 @@
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
     </row>
-    <row r="23" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>

</xml_diff>

<commit_message>
Finished modification of config file. Changed the name of parameters sheet
</commit_message>
<xml_diff>
--- a/PWC. Шаблоны входа робота.xlsx
+++ b/PWC. Шаблоны входа робота.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\PwC\PwC-Aeroflot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D527939-193B-4938-9E56-600B92B678B2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9263BC97-E00B-4DDC-BC81-768C7CD266FA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4644" yWindow="456" windowWidth="28800" windowHeight="15984" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Инструкция" sheetId="5" r:id="rId1"/>
-    <sheet name="Params" sheetId="4" r:id="rId2"/>
+    <sheet name="Параметры" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="70">
   <si>
     <t>Расстояние</t>
   </si>
@@ -191,9 +191,6 @@
     <t>Краткое описание шага</t>
   </si>
   <si>
-    <t>STReadConfiguration</t>
-  </si>
-  <si>
     <t>Выполнить чтение конфигурации</t>
   </si>
   <si>
@@ -203,161 +200,6 @@
     <t>+</t>
   </si>
   <si>
-    <t>Выполнить загрузку конфигурационного файла в переменные</t>
-  </si>
-  <si>
-    <t>STValidateConfiguration</t>
-  </si>
-  <si>
-    <t>Выполнить валидацию входящих данных</t>
-  </si>
-  <si>
-    <t>Выполнить всевозможную валидацию всего, что только можно: проверить наличие всех входных/выходных файлов и папок. Проверить структуры ОСВ и т.д.</t>
-  </si>
-  <si>
-    <t>STPrepareStatus</t>
-  </si>
-  <si>
-    <t>Выполнить формирование статусного файла</t>
-  </si>
-  <si>
-    <t>Сформировать рыбу статусного файла Status.xlsm, который должен лежать в корне Output folder. Внимание: При формировании статусного файла используется VBA код (STPrepareStatus), хранимый в конфигурационном файле.</t>
-  </si>
-  <si>
-    <t>AOpenSAP</t>
-  </si>
-  <si>
-    <t>Выполнить вход в SAP</t>
-  </si>
-  <si>
-    <t>Главное меню SAP</t>
-  </si>
-  <si>
-    <t>STProcessRow</t>
-  </si>
-  <si>
-    <t>Циклическая отработка строк конфигурации</t>
-  </si>
-  <si>
-    <t>Выполнить обработку строки конфигурации: подготовить файловую структуру, запустить процесс циклической технической выгрузки
-Сформировать/проверить наличие папки группы
-Сформировать/проверить наличие файла выгрузки</t>
-  </si>
-  <si>
-    <t>STProcessRowSTExportSAP</t>
-  </si>
-  <si>
-    <t>Циклическая выгрузка технических файликов</t>
-  </si>
-  <si>
-    <t>STProcessRowSTExportSAPAExportPart</t>
-  </si>
-  <si>
-    <t>Выполнить выгрузку части данных</t>
-  </si>
-  <si>
-    <t>Зайти в транзакцию, установить параметры, запустить формирование, выполнить экспорт и сохранить Excel файл на диск</t>
-  </si>
-  <si>
-    <t>STProcessRowACombineTechPart</t>
-  </si>
-  <si>
-    <t>Добавить выгруженные данные в основной файл</t>
-  </si>
-  <si>
-    <t>Выполнить объединение технических файлов в один.+Подтягивание списка ВГО контрагентов. +Подтягивание ОСВ. При выполнении операции используется VBA код STProcessRowACombineTechPart</t>
-  </si>
-  <si>
-    <t>STProcessRowARecalculateRowFile</t>
-  </si>
-  <si>
-    <t>Выполнить обсчет файла</t>
-  </si>
-  <si>
-    <t>Выполнить расчет Excel файла: расчет доп. колонок в выгрузке; расчет доп. Колонки в ОСВ (код счета); Обновлние пивота ОСВСвод; Обновление пивота Сверка; Обновление пивота Свод   При выполнении операции используется VBA код STProcessRowARecalculateRowFile</t>
-  </si>
-  <si>
-    <t>STProcessGroup</t>
-  </si>
-  <si>
-    <t>Циклическая отработка групп</t>
-  </si>
-  <si>
-    <t>STProcessGroupAUpdateGroupFile</t>
-  </si>
-  <si>
-    <t>Сформировать/проверить файл группы</t>
-  </si>
-  <si>
-    <t>STProcessGroupSTProcessRowFile</t>
-  </si>
-  <si>
-    <t>Циклическая обработка основных файлов группы</t>
-  </si>
-  <si>
-    <t>STProcessGroupSTProcessRowFileAAddToGroupFile</t>
-  </si>
-  <si>
-    <t>Скопировать данные из вкладки Свод основного файла строки и добавить в конец вкладки Свод файла группы</t>
-  </si>
-  <si>
-    <t>STProcessGroupSTProcessRowFileAProcessGroupFile</t>
-  </si>
-  <si>
-    <t>Обработать групповой файл</t>
-  </si>
-  <si>
-    <t>STPrepareStatusASetData</t>
-  </si>
-  <si>
-    <t>Вывести информацию о статусе обработки в файл</t>
-  </si>
-  <si>
-    <t>ACloseSAP</t>
-  </si>
-  <si>
-    <t>Закрыть SAP</t>
-  </si>
-  <si>
-    <t>Закрыть приложение SAP</t>
-  </si>
-  <si>
-    <t>ADisconnectVPN</t>
-  </si>
-  <si>
-    <t>Выключить VPN</t>
-  </si>
-  <si>
-    <t>Закрыть VPN соединение</t>
-  </si>
-  <si>
-    <t>AConnectVPN</t>
-  </si>
-  <si>
-    <t>Включить VPN</t>
-  </si>
-  <si>
-    <t>Открыть VPN соединение</t>
-  </si>
-  <si>
-    <t>AConnectWiFi</t>
-  </si>
-  <si>
-    <t>Включить WiFi</t>
-  </si>
-  <si>
-    <t>Открыть WiFi соединение</t>
-  </si>
-  <si>
-    <t>TEstablishConnection</t>
-  </si>
-  <si>
-    <t>Установка соединения</t>
-  </si>
-  <si>
-    <t>Установить необходимое соединение (на случай, если наблюдаются проблемы с доступом)</t>
-  </si>
-  <si>
     <t>Заходим на сайт "Аэрофлота" https://www.aeroflot.ru/ikm/, вводим данные о перелетах по направлениям из входного файла, считываем данные о бонусныхбаллах за данные перелеты и сохраняем в выходной файл</t>
   </si>
   <si>
@@ -365,6 +207,30 @@
   </si>
   <si>
     <t>Перед запуском рекомендуется закрыть все окна Excel и Chrome. После запуска робот самостоятельно выполнит следующие действия: откроет конфигурационный файл Excel, прочитает входные параметры, откроет страницу браузера на сайте компании "Аэрофлот", выполнит выгрузку данных с сайта, обработает данные и сохранит результат работы в Excel</t>
+  </si>
+  <si>
+    <t>StReadConfiguration</t>
+  </si>
+  <si>
+    <t>StDataProcess</t>
+  </si>
+  <si>
+    <t>Обработать данные</t>
+  </si>
+  <si>
+    <t>StWriteResultData</t>
+  </si>
+  <si>
+    <t>Запись результатов в файл</t>
+  </si>
+  <si>
+    <t>Выполняет загрузку конфигурационного файла в переменные</t>
+  </si>
+  <si>
+    <t>Заполняет форму на сайте прочитанными данными и считывает количество миль для каждого перелета</t>
+  </si>
+  <si>
+    <t>Копирует исходный файл конфигураций, добавляет столбец "Статус сверки", обновляет данные в таблице о бонусных милях и указывает статус сверки</t>
   </si>
 </sst>
 </file>
@@ -458,21 +324,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <color theme="5"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -488,6 +339,21 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="9"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
@@ -620,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -683,35 +549,38 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1330,7 +1199,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1360,7 +1229,7 @@
         <v>42</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>111</v>
+        <v>59</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -1384,7 +1253,7 @@
         <v>44</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>113</v>
+        <v>61</v>
       </c>
       <c r="C4" s="19"/>
       <c r="D4" s="19"/>
@@ -1392,7 +1261,7 @@
       <c r="F4" s="19"/>
     </row>
     <row r="5" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="26" t="s">
         <v>45</v>
       </c>
       <c r="B5" s="21" t="s">
@@ -1404,9 +1273,9 @@
       <c r="F5" s="19"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
+      <c r="A6" s="26"/>
       <c r="B6" s="19" t="s">
-        <v>112</v>
+        <v>60</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
@@ -1464,396 +1333,207 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="C11" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="D11" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="F11" s="35" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="31.2" x14ac:dyDescent="0.25">
+      <c r="A12" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="F11" s="26" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" s="28" t="s">
+      <c r="F12" s="35" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A13" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="28" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="61.8" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="C13" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="F13" s="26" t="s">
-        <v>66</v>
+      <c r="F13" s="35" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="B14" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="E14" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="F14" s="26" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="51.6" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="B15" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="C15" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="E15" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="F15" s="26" t="s">
-        <v>72</v>
-      </c>
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="27"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="27"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="B16" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="D16" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="F16" s="23"/>
-    </row>
-    <row r="17" spans="1:6" ht="31.2" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="B17" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="C17" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="E17" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="F17" s="26" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="51.6" x14ac:dyDescent="0.25">
-      <c r="A18" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="B18" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="C18" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="D18" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="E18" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="F18" s="26" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="61.8" x14ac:dyDescent="0.25">
-      <c r="A19" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="B19" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="C19" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="D19" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="E19" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="F19" s="26" t="s">
-        <v>83</v>
-      </c>
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="29"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="27"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="27"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="27"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="B20" s="31" t="s">
-        <v>85</v>
-      </c>
-      <c r="C20" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="D20" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" s="32" t="s">
-        <v>11</v>
-      </c>
+      <c r="A20" s="31"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="32"/>
       <c r="F20" s="31"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="B21" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="C21" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="D21" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="E21" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="23"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="29"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="B22" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="C22" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="E22" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="23"/>
-    </row>
-    <row r="23" spans="1:6" ht="31.2" x14ac:dyDescent="0.25">
-      <c r="A23" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="B23" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="C23" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="D23" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="E23" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" s="23"/>
-    </row>
-    <row r="24" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="A24" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="B24" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="C24" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="D24" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="E24" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" s="23"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="29"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="29"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="29"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="29"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="29"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="B25" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="C25" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="D25" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="E25" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25" s="23"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="29"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="B26" s="26" t="s">
-        <v>97</v>
-      </c>
-      <c r="C26" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="D26" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="E26" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="F26" s="26" t="s">
-        <v>98</v>
-      </c>
+      <c r="A26" s="27"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="27"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="26" t="s">
-        <v>99</v>
-      </c>
-      <c r="B27" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="C27" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="D27" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="E27" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="F27" s="26" t="s">
-        <v>101</v>
-      </c>
+      <c r="A27" s="27"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="27"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="B28" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="C28" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="D28" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="E28" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="F28" s="26" t="s">
-        <v>104</v>
-      </c>
+      <c r="A28" s="27"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="27"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="B29" s="26" t="s">
-        <v>106</v>
-      </c>
-      <c r="C29" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="D29" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="E29" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="F29" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="A30" s="26" t="s">
-        <v>108</v>
-      </c>
-      <c r="B30" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="C30" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="D30" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="E30" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="F30" s="26" t="s">
-        <v>110</v>
-      </c>
+      <c r="A29" s="27"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="27"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="27"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A5:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add 3 steps in config file
</commit_message>
<xml_diff>
--- a/PWC. Шаблоны входа робота.xlsx
+++ b/PWC. Шаблоны входа робота.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\PwC\PwC-Aeroflot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vietnguyen/Downloads/PwC-Aeroflot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9263BC97-E00B-4DDC-BC81-768C7CD266FA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93890465-5357-F94F-B5E0-F46F097BCC0A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4644" yWindow="456" windowWidth="28800" windowHeight="15984" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Инструкция" sheetId="5" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="80">
   <si>
     <t>Расстояние</t>
   </si>
@@ -231,6 +231,36 @@
   </si>
   <si>
     <t>Копирует исходный файл конфигураций, добавляет столбец "Статус сверки", обновляет данные в таблице о бонусных милях и указывает статус сверки</t>
+  </si>
+  <si>
+    <t>InputValuesInBrower</t>
+  </si>
+  <si>
+    <t>Ввод данных на сайте Аэрофлота</t>
+  </si>
+  <si>
+    <t>Веб-страница Аэрофлот</t>
+  </si>
+  <si>
+    <t>Заполняет форму на сайте</t>
+  </si>
+  <si>
+    <t>ValidationsCells</t>
+  </si>
+  <si>
+    <t>Проверка введенных данных</t>
+  </si>
+  <si>
+    <t>Проверяет правильно ли введенны исходные данные и ожидает пока таблица с данными на сайте обновится</t>
+  </si>
+  <si>
+    <t>GettingResults</t>
+  </si>
+  <si>
+    <t>Получение результата</t>
+  </si>
+  <si>
+    <t>Получает результат с таблицы</t>
   </si>
 </sst>
 </file>
@@ -486,7 +516,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -549,42 +579,48 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
@@ -900,9 +936,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -940,7 +976,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1046,7 +1082,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1196,23 +1232,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39BFAB1C-68A9-4038-9886-24B2DD8AE8D1}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="34.88671875" customWidth="1"/>
-    <col min="2" max="2" width="35.21875" customWidth="1"/>
-    <col min="3" max="3" width="25.109375" customWidth="1"/>
+    <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="2" max="2" width="35.1640625" customWidth="1"/>
+    <col min="3" max="3" width="25.1640625" customWidth="1"/>
     <col min="4" max="4" width="24.33203125" customWidth="1"/>
-    <col min="5" max="5" width="23.44140625" customWidth="1"/>
+    <col min="5" max="5" width="23.5" customWidth="1"/>
     <col min="6" max="6" width="35.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="18" t="s">
         <v>40</v>
       </c>
@@ -1224,7 +1260,7 @@
       <c r="E1" s="19"/>
       <c r="F1" s="19"/>
     </row>
-    <row r="2" spans="1:6" ht="51" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.15">
       <c r="A2" s="18" t="s">
         <v>42</v>
       </c>
@@ -1236,7 +1272,7 @@
       <c r="E2" s="19"/>
       <c r="F2" s="19"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="18" t="s">
         <v>43</v>
       </c>
@@ -1248,7 +1284,7 @@
       <c r="E3" s="19"/>
       <c r="F3" s="19"/>
     </row>
-    <row r="4" spans="1:6" ht="82.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="96" x14ac:dyDescent="0.15">
       <c r="A4" s="18" t="s">
         <v>44</v>
       </c>
@@ -1260,8 +1296,8 @@
       <c r="E4" s="19"/>
       <c r="F4" s="19"/>
     </row>
-    <row r="5" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+    <row r="5" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+      <c r="A5" s="36" t="s">
         <v>45</v>
       </c>
       <c r="B5" s="21" t="s">
@@ -1272,8 +1308,8 @@
       <c r="E5" s="19"/>
       <c r="F5" s="19"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" s="36"/>
       <c r="B6" s="19" t="s">
         <v>60</v>
       </c>
@@ -1282,7 +1318,7 @@
       <c r="E6" s="19"/>
       <c r="F6" s="19"/>
     </row>
-    <row r="7" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A7" s="18" t="s">
         <v>47</v>
       </c>
@@ -1294,7 +1330,7 @@
       <c r="E7" s="19"/>
       <c r="F7" s="19"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="19"/>
       <c r="B8" s="19"/>
       <c r="C8" s="19"/>
@@ -1302,7 +1338,7 @@
       <c r="E8" s="19"/>
       <c r="F8" s="19"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="22" t="s">
         <v>49</v>
       </c>
@@ -1312,7 +1348,7 @@
       <c r="E9" s="23"/>
       <c r="F9" s="23"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="24" t="s">
         <v>50</v>
       </c>
@@ -1332,201 +1368,261 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
+    <row r="11" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+      <c r="A11" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="C11" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="35" t="s">
+      <c r="D11" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="36" t="s">
+      <c r="E11" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="35" t="s">
+      <c r="F11" s="34" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="31.2" x14ac:dyDescent="0.25">
-      <c r="A12" s="35" t="s">
+    <row r="12" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+      <c r="A12" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="36" t="s">
+      <c r="E12" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="35" t="s">
+      <c r="F12" s="34" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A13" s="35" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+      <c r="A14" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="34" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A15" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="34" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+      <c r="A16" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B16" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C16" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="35" t="s">
+      <c r="D16" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="36" t="s">
+      <c r="E16" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="35" t="s">
+      <c r="F16" s="34" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="27"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="27"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="29"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="27"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="27"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="27"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="31"/>
-      <c r="B20" s="31"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="31"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="29"/>
-      <c r="B21" s="29"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="29"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="29"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="29"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="29"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="29"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="29"/>
-      <c r="B24" s="29"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="29"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="29"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="29"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="27"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="27"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="27"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="27"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="27"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="27"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="27"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="27"/>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="26"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="26"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="28"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A20" s="26"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="26"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A21" s="26"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="26"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A22" s="26"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="26"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A23" s="30"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="30"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A24" s="28"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="28"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A25" s="28"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="28"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A26" s="28"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="28"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A27" s="28"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="28"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A28" s="28"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="28"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A29" s="26"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="26"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A30" s="26"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="26"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A31" s="26"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="26"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A32" s="26"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="26"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A33" s="26"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1545,22 +1641,22 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="179" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" customWidth="1"/>
     <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -1586,7 +1682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -1612,7 +1708,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
@@ -1638,7 +1734,7 @@
         <v>11506</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
@@ -1654,7 +1750,7 @@
       <c r="G4" s="16"/>
       <c r="H4" s="12"/>
     </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="9" t="s">
         <v>1</v>
       </c>
@@ -1680,7 +1776,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="9" t="s">
         <v>35</v>
       </c>
@@ -1704,7 +1800,7 @@
       </c>
       <c r="H6" s="12"/>
     </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="9" t="s">
         <v>1</v>
       </c>
@@ -1728,7 +1824,7 @@
       </c>
       <c r="H7" s="12"/>
     </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="9" t="s">
         <v>1</v>
       </c>
@@ -1752,7 +1848,7 @@
       </c>
       <c r="H8" s="12"/>
     </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="9" t="s">
         <v>1</v>
       </c>
@@ -1778,7 +1874,7 @@
         <v>24484</v>
       </c>
     </row>
-    <row r="20" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -1789,7 +1885,7 @@
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
     </row>
-    <row r="21" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F21" s="3"/>
       <c r="G21" s="4"/>
       <c r="H21" s="5"/>
@@ -1800,7 +1896,7 @@
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
     </row>
-    <row r="22" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -1811,7 +1907,7 @@
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
     </row>
-    <row r="23" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>

</xml_diff>

<commit_message>
Changed robot code. Spellchecked config file
</commit_message>
<xml_diff>
--- a/PWC. Шаблоны входа робота.xlsx
+++ b/PWC. Шаблоны входа робота.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vietnguyen/Downloads/PwC-Aeroflot/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\PwC\PwC-Aeroflot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93890465-5357-F94F-B5E0-F46F097BCC0A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA20F40-04B9-40BF-8D77-AC903F556843}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="28800" windowHeight="15984" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Инструкция" sheetId="5" r:id="rId1"/>
@@ -146,15 +146,9 @@
     <t>Код робота</t>
   </si>
   <si>
-    <t>R2 (Тест + Аналитика)</t>
-  </si>
-  <si>
     <t>Описание робота</t>
   </si>
   <si>
-    <t>Ипользуемые транзакции SAP</t>
-  </si>
-  <si>
     <t>Как запустить робота?</t>
   </si>
   <si>
@@ -200,9 +194,6 @@
     <t>+</t>
   </si>
   <si>
-    <t>Заходим на сайт "Аэрофлота" https://www.aeroflot.ru/ikm/, вводим данные о перелетах по направлениям из входного файла, считываем данные о бонусныхбаллах за данные перелеты и сохраняем в выходной файл</t>
-  </si>
-  <si>
     <t>файл конфигурации в формате *.xlsx</t>
   </si>
   <si>
@@ -251,9 +242,6 @@
     <t>Проверка введенных данных</t>
   </si>
   <si>
-    <t>Проверяет правильно ли введенны исходные данные и ожидает пока таблица с данными на сайте обновится</t>
-  </si>
-  <si>
     <t>GettingResults</t>
   </si>
   <si>
@@ -261,6 +249,18 @@
   </si>
   <si>
     <t>Получает результат с таблицы</t>
+  </si>
+  <si>
+    <t>Проверяет правильно ли введены исходные данные и ожидает пока таблица с данными на сайте обновится</t>
+  </si>
+  <si>
+    <t>Заходим на сайт "Аэрофлота" https://www.aeroflot.ru/ikm/, вводим данные о перелетах по направлениям из входного файла, считываем данные о бонусных баллах за данные перелеты и сохраняем в выходной файл</t>
+  </si>
+  <si>
+    <t>Используемые транзакции SAP</t>
+  </si>
+  <si>
+    <t>R34 AFL</t>
   </si>
 </sst>
 </file>
@@ -609,18 +609,18 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
@@ -936,9 +936,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -976,7 +976,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1082,7 +1082,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1234,47 +1234,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39BFAB1C-68A9-4038-9886-24B2DD8AE8D1}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.83203125" customWidth="1"/>
-    <col min="2" max="2" width="35.1640625" customWidth="1"/>
-    <col min="3" max="3" width="25.1640625" customWidth="1"/>
+    <col min="1" max="1" width="34.77734375" customWidth="1"/>
+    <col min="2" max="2" width="35.109375" customWidth="1"/>
+    <col min="3" max="3" width="25.109375" customWidth="1"/>
     <col min="4" max="4" width="24.33203125" customWidth="1"/>
-    <col min="5" max="5" width="23.5" customWidth="1"/>
+    <col min="5" max="5" width="23.44140625" customWidth="1"/>
     <col min="6" max="6" width="35.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>40</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
       <c r="E1" s="19"/>
       <c r="F1" s="19"/>
     </row>
-    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="51" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
       <c r="E2" s="19"/>
       <c r="F2" s="19"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>11</v>
@@ -1284,53 +1284,53 @@
       <c r="E3" s="19"/>
       <c r="F3" s="19"/>
     </row>
-    <row r="4" spans="1:6" ht="96" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="82.2" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C4" s="19"/>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
       <c r="F4" s="19"/>
     </row>
-    <row r="5" spans="1:6" ht="24" x14ac:dyDescent="0.15">
-      <c r="A5" s="36" t="s">
-        <v>45</v>
+    <row r="5" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="38" t="s">
+        <v>43</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
       <c r="F5" s="19"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="36"/>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="38"/>
       <c r="B6" s="19" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
       <c r="E6" s="19"/>
       <c r="F6" s="19"/>
     </row>
-    <row r="7" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C7" s="19"/>
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
       <c r="F7" s="19"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="19"/>
       <c r="B8" s="19"/>
       <c r="C8" s="19"/>
@@ -1338,9 +1338,9 @@
       <c r="E8" s="19"/>
       <c r="F8" s="19"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
@@ -1348,147 +1348,147 @@
       <c r="E9" s="23"/>
       <c r="F9" s="23"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="D10" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="E10" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="F10" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="25" t="s">
+    </row>
+    <row r="11" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="C11" s="34" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="24" x14ac:dyDescent="0.15">
-      <c r="A11" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="34" t="s">
+      <c r="D11" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" s="35" t="s">
-        <v>58</v>
-      </c>
       <c r="F11" s="34" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="31.2" x14ac:dyDescent="0.25">
+      <c r="A12" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="36" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="24" x14ac:dyDescent="0.15">
-      <c r="A12" s="34" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="C12" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12" s="34" t="s">
+      <c r="B13" s="34" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" s="37" t="s">
+      <c r="C13" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="B13" s="34" t="s">
+    </row>
+    <row r="14" spans="1:6" ht="31.2" x14ac:dyDescent="0.25">
+      <c r="A14" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="B14" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="D13" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="E13" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="F13" s="34" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="24" x14ac:dyDescent="0.15">
-      <c r="A14" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="B14" s="34" t="s">
-        <v>75</v>
-      </c>
       <c r="C14" s="34" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="E14" s="38" t="s">
-        <v>58</v>
+        <v>69</v>
+      </c>
+      <c r="E14" s="37" t="s">
+        <v>56</v>
       </c>
       <c r="F14" s="34" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" s="37" t="s">
-        <v>77</v>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="36" t="s">
+        <v>73</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" s="38" t="s">
-        <v>58</v>
+        <v>69</v>
+      </c>
+      <c r="E15" s="37" t="s">
+        <v>56</v>
       </c>
       <c r="F15" s="34" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A16" s="34" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B16" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="D16" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="F16" s="34" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="26"/>
       <c r="B17" s="26"/>
       <c r="C17" s="26"/>
@@ -1496,7 +1496,7 @@
       <c r="E17" s="27"/>
       <c r="F17" s="26"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="26"/>
       <c r="B18" s="26"/>
       <c r="C18" s="26"/>
@@ -1504,7 +1504,7 @@
       <c r="E18" s="27"/>
       <c r="F18" s="26"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="26"/>
       <c r="B19" s="26"/>
       <c r="C19" s="26"/>
@@ -1512,7 +1512,7 @@
       <c r="E19" s="27"/>
       <c r="F19" s="28"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="26"/>
       <c r="B20" s="26"/>
       <c r="C20" s="26"/>
@@ -1520,7 +1520,7 @@
       <c r="E20" s="29"/>
       <c r="F20" s="26"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="26"/>
       <c r="B21" s="26"/>
       <c r="C21" s="26"/>
@@ -1528,7 +1528,7 @@
       <c r="E21" s="27"/>
       <c r="F21" s="26"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="26"/>
       <c r="B22" s="26"/>
       <c r="C22" s="26"/>
@@ -1536,7 +1536,7 @@
       <c r="E22" s="27"/>
       <c r="F22" s="26"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="30"/>
       <c r="B23" s="30"/>
       <c r="C23" s="30"/>
@@ -1544,7 +1544,7 @@
       <c r="E23" s="31"/>
       <c r="F23" s="30"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="28"/>
       <c r="B24" s="28"/>
       <c r="C24" s="32"/>
@@ -1552,7 +1552,7 @@
       <c r="E24" s="33"/>
       <c r="F24" s="28"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="28"/>
       <c r="B25" s="28"/>
       <c r="C25" s="32"/>
@@ -1560,7 +1560,7 @@
       <c r="E25" s="33"/>
       <c r="F25" s="28"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="28"/>
       <c r="B26" s="28"/>
       <c r="C26" s="32"/>
@@ -1568,7 +1568,7 @@
       <c r="E26" s="33"/>
       <c r="F26" s="28"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="28"/>
       <c r="B27" s="28"/>
       <c r="C27" s="32"/>
@@ -1576,7 +1576,7 @@
       <c r="E27" s="33"/>
       <c r="F27" s="28"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="28"/>
       <c r="B28" s="28"/>
       <c r="C28" s="32"/>
@@ -1584,7 +1584,7 @@
       <c r="E28" s="33"/>
       <c r="F28" s="28"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="26"/>
       <c r="B29" s="26"/>
       <c r="C29" s="26"/>
@@ -1592,7 +1592,7 @@
       <c r="E29" s="27"/>
       <c r="F29" s="26"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="26"/>
       <c r="B30" s="26"/>
       <c r="C30" s="26"/>
@@ -1600,7 +1600,7 @@
       <c r="E30" s="27"/>
       <c r="F30" s="26"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="26"/>
       <c r="B31" s="26"/>
       <c r="C31" s="26"/>
@@ -1608,7 +1608,7 @@
       <c r="E31" s="27"/>
       <c r="F31" s="26"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="26"/>
       <c r="B32" s="26"/>
       <c r="C32" s="26"/>
@@ -1616,7 +1616,7 @@
       <c r="E32" s="27"/>
       <c r="F32" s="26"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="26"/>
       <c r="B33" s="26"/>
       <c r="C33" s="26"/>
@@ -1640,23 +1640,23 @@
   </sheetPr>
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="179" workbookViewId="0">
+    <sheetView zoomScale="179" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
     <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
@@ -1734,7 +1734,7 @@
         <v>11506</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
@@ -1750,7 +1750,7 @@
       <c r="G4" s="16"/>
       <c r="H4" s="12"/>
     </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>1</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>35</v>
       </c>
@@ -1800,7 +1800,7 @@
       </c>
       <c r="H6" s="12"/>
     </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>1</v>
       </c>
@@ -1824,7 +1824,7 @@
       </c>
       <c r="H7" s="12"/>
     </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>1</v>
       </c>
@@ -1848,7 +1848,7 @@
       </c>
       <c r="H8" s="12"/>
     </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>1</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>24484</v>
       </c>
     </row>
-    <row r="20" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -1885,7 +1885,7 @@
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
     </row>
-    <row r="21" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F21" s="3"/>
       <c r="G21" s="4"/>
       <c r="H21" s="5"/>
@@ -1896,7 +1896,7 @@
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
     </row>
-    <row r="22" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -1907,7 +1907,7 @@
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
     </row>
-    <row r="23" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>

</xml_diff>